<commit_message>
adding template excel file
</commit_message>
<xml_diff>
--- a/7_ALM/FetchALMDataToSmartsheet/Data/template.xlsx
+++ b/7_ALM/FetchALMDataToSmartsheet/Data/template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -29,6 +29,12 @@
       <b val="1"/>
       <color theme="1"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="BatangChe"/>
+      <charset val="129"/>
+      <family val="3"/>
+      <sz val="8"/>
     </font>
   </fonts>
   <fills count="4">
@@ -147,7 +153,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -525,39 +531,39 @@
   <dimension ref="A1:AD682"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="Z1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1"/>
+      <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col width="10.140625" customWidth="1" min="1" max="1"/>
-    <col width="9.28515625" customWidth="1" min="2" max="2"/>
-    <col width="81.7109375" customWidth="1" min="3" max="3"/>
-    <col hidden="1" width="16.5703125" customWidth="1" min="4" max="4"/>
-    <col hidden="1" width="20.42578125" customWidth="1" min="5" max="5"/>
-    <col hidden="1" width="24.5703125" customWidth="1" min="6" max="6"/>
-    <col hidden="1" width="15.7109375" customWidth="1" min="7" max="7"/>
-    <col hidden="1" width="19.7109375" customWidth="1" min="8" max="8"/>
-    <col hidden="1" width="10.85546875" customWidth="1" min="9" max="9"/>
-    <col width="19.7109375" customWidth="1" min="10" max="10"/>
-    <col hidden="1" width="14.5703125" customWidth="1" min="11" max="11"/>
-    <col hidden="1" width="13.28515625" customWidth="1" min="12" max="12"/>
-    <col width="10.7109375" customWidth="1" min="13" max="13"/>
-    <col width="16.85546875" customWidth="1" min="14" max="14"/>
+    <col width="10.109375" customWidth="1" min="1" max="1"/>
+    <col width="9.33203125" customWidth="1" min="2" max="2"/>
+    <col width="81.6640625" customWidth="1" min="3" max="3"/>
+    <col hidden="1" width="16.5546875" customWidth="1" min="4" max="4"/>
+    <col hidden="1" width="20.44140625" customWidth="1" min="5" max="5"/>
+    <col hidden="1" width="24.5546875" customWidth="1" min="6" max="6"/>
+    <col hidden="1" width="15.6640625" customWidth="1" min="7" max="7"/>
+    <col hidden="1" width="19.6640625" customWidth="1" min="8" max="8"/>
+    <col hidden="1" width="10.88671875" customWidth="1" min="9" max="9"/>
+    <col width="19.6640625" customWidth="1" min="10" max="10"/>
+    <col hidden="1" width="14.5546875" customWidth="1" min="11" max="11"/>
+    <col hidden="1" width="13.33203125" customWidth="1" min="12" max="12"/>
+    <col width="10.6640625" customWidth="1" min="13" max="13"/>
+    <col width="16.88671875" customWidth="1" min="14" max="14"/>
     <col hidden="1" width="26" customWidth="1" min="15" max="15"/>
-    <col hidden="1" width="17.28515625" customWidth="1" min="16" max="16"/>
-    <col hidden="1" width="15.42578125" customWidth="1" min="17" max="17"/>
-    <col hidden="1" width="20.28515625" customWidth="1" min="18" max="18"/>
-    <col width="40.140625" customWidth="1" min="19" max="19"/>
-    <col hidden="1" width="12.140625" customWidth="1" min="20" max="20"/>
-    <col hidden="1" width="16.85546875" customWidth="1" min="21" max="21"/>
-    <col hidden="1" width="38.7109375" customWidth="1" min="22" max="22"/>
+    <col hidden="1" width="17.33203125" customWidth="1" min="16" max="16"/>
+    <col hidden="1" width="15.44140625" customWidth="1" min="17" max="17"/>
+    <col hidden="1" width="20.33203125" customWidth="1" min="18" max="18"/>
+    <col width="40.109375" customWidth="1" min="19" max="19"/>
+    <col hidden="1" width="12.109375" customWidth="1" min="20" max="20"/>
+    <col hidden="1" width="16.88671875" customWidth="1" min="21" max="21"/>
+    <col hidden="1" width="38.6640625" customWidth="1" min="22" max="22"/>
     <col hidden="1" width="13" customWidth="1" min="23" max="23"/>
-    <col hidden="1" width="11.28515625" customWidth="1" min="24" max="24"/>
-    <col width="30.28515625" customWidth="1" min="25" max="25"/>
-    <col width="38.28515625" customWidth="1" min="26" max="26"/>
-    <col width="94.7109375" customWidth="1" min="27" max="27"/>
-    <col width="34.140625" customWidth="1" min="28" max="28"/>
+    <col hidden="1" width="11.33203125" customWidth="1" min="24" max="24"/>
+    <col width="30.33203125" customWidth="1" min="25" max="25"/>
+    <col width="38.33203125" customWidth="1" min="26" max="26"/>
+    <col width="94.6640625" customWidth="1" min="27" max="27"/>
+    <col width="34.109375" customWidth="1" min="28" max="28"/>
     <col width="13" customWidth="1" min="29" max="30"/>
   </cols>
   <sheetData>
@@ -866,6 +872,9 @@
 ======================================================================</t>
         </is>
       </c>
+      <c r="AB2" s="2" t="n"/>
+      <c r="AC2" s="2" t="n"/>
+      <c r="AD2" s="2" t="n"/>
     </row>
     <row r="3" ht="15" customHeight="1">
       <c r="A3" s="3" t="n"/>
@@ -895,6 +904,9 @@
       <c r="Y3" s="3" t="n"/>
       <c r="Z3" s="3" t="n"/>
       <c r="AA3" s="3" t="n"/>
+      <c r="AB3" s="3" t="n"/>
+      <c r="AC3" s="3" t="n"/>
+      <c r="AD3" s="3" t="n"/>
     </row>
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="4" t="n"/>
@@ -924,6 +936,9 @@
       <c r="Y4" s="4" t="n"/>
       <c r="Z4" s="4" t="n"/>
       <c r="AA4" s="4" t="n"/>
+      <c r="AB4" s="4" t="n"/>
+      <c r="AC4" s="4" t="n"/>
+      <c r="AD4" s="4" t="n"/>
     </row>
     <row r="5" ht="15" customHeight="1">
       <c r="A5" s="3" t="n"/>
@@ -953,6 +968,9 @@
       <c r="Y5" s="3" t="n"/>
       <c r="Z5" s="3" t="n"/>
       <c r="AA5" s="3" t="n"/>
+      <c r="AB5" s="3" t="n"/>
+      <c r="AC5" s="3" t="n"/>
+      <c r="AD5" s="3" t="n"/>
     </row>
     <row r="6" ht="15" customHeight="1">
       <c r="A6" s="4" t="n"/>
@@ -982,6 +1000,9 @@
       <c r="Y6" s="4" t="n"/>
       <c r="Z6" s="4" t="n"/>
       <c r="AA6" s="4" t="n"/>
+      <c r="AB6" s="4" t="n"/>
+      <c r="AC6" s="4" t="n"/>
+      <c r="AD6" s="4" t="n"/>
     </row>
     <row r="7" ht="15" customHeight="1">
       <c r="A7" s="3" t="n"/>
@@ -1011,6 +1032,9 @@
       <c r="Y7" s="3" t="n"/>
       <c r="Z7" s="3" t="n"/>
       <c r="AA7" s="3" t="n"/>
+      <c r="AB7" s="3" t="n"/>
+      <c r="AC7" s="3" t="n"/>
+      <c r="AD7" s="3" t="n"/>
     </row>
     <row r="8" ht="15" customHeight="1">
       <c r="A8" s="4" t="n"/>
@@ -1040,6 +1064,9 @@
       <c r="Y8" s="4" t="n"/>
       <c r="Z8" s="4" t="n"/>
       <c r="AA8" s="4" t="n"/>
+      <c r="AB8" s="4" t="n"/>
+      <c r="AC8" s="4" t="n"/>
+      <c r="AD8" s="4" t="n"/>
     </row>
     <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3" t="n"/>
@@ -1069,6 +1096,9 @@
       <c r="Y9" s="3" t="n"/>
       <c r="Z9" s="3" t="n"/>
       <c r="AA9" s="3" t="n"/>
+      <c r="AB9" s="3" t="n"/>
+      <c r="AC9" s="3" t="n"/>
+      <c r="AD9" s="3" t="n"/>
     </row>
     <row r="10" ht="15" customHeight="1">
       <c r="A10" s="4" t="n"/>
@@ -1098,6 +1128,9 @@
       <c r="Y10" s="4" t="n"/>
       <c r="Z10" s="4" t="n"/>
       <c r="AA10" s="4" t="n"/>
+      <c r="AB10" s="4" t="n"/>
+      <c r="AC10" s="4" t="n"/>
+      <c r="AD10" s="4" t="n"/>
     </row>
     <row r="11" ht="15" customHeight="1">
       <c r="A11" s="3" t="n"/>
@@ -1127,6 +1160,9 @@
       <c r="Y11" s="3" t="n"/>
       <c r="Z11" s="3" t="n"/>
       <c r="AA11" s="3" t="n"/>
+      <c r="AB11" s="3" t="n"/>
+      <c r="AC11" s="3" t="n"/>
+      <c r="AD11" s="3" t="n"/>
     </row>
     <row r="12" ht="15" customHeight="1">
       <c r="A12" s="4" t="n"/>
@@ -1156,6 +1192,9 @@
       <c r="Y12" s="4" t="n"/>
       <c r="Z12" s="4" t="n"/>
       <c r="AA12" s="4" t="n"/>
+      <c r="AB12" s="4" t="n"/>
+      <c r="AC12" s="4" t="n"/>
+      <c r="AD12" s="4" t="n"/>
     </row>
     <row r="13" ht="15" customHeight="1">
       <c r="A13" s="3" t="n"/>
@@ -1185,6 +1224,9 @@
       <c r="Y13" s="3" t="n"/>
       <c r="Z13" s="3" t="n"/>
       <c r="AA13" s="3" t="n"/>
+      <c r="AB13" s="3" t="n"/>
+      <c r="AC13" s="3" t="n"/>
+      <c r="AD13" s="3" t="n"/>
     </row>
     <row r="14" ht="15" customHeight="1">
       <c r="A14" s="4" t="n"/>
@@ -1214,6 +1256,9 @@
       <c r="Y14" s="4" t="n"/>
       <c r="Z14" s="4" t="n"/>
       <c r="AA14" s="4" t="n"/>
+      <c r="AB14" s="4" t="n"/>
+      <c r="AC14" s="4" t="n"/>
+      <c r="AD14" s="4" t="n"/>
     </row>
     <row r="15" ht="15" customHeight="1">
       <c r="A15" s="3" t="n"/>
@@ -1243,6 +1288,9 @@
       <c r="Y15" s="3" t="n"/>
       <c r="Z15" s="3" t="n"/>
       <c r="AA15" s="3" t="n"/>
+      <c r="AB15" s="3" t="n"/>
+      <c r="AC15" s="3" t="n"/>
+      <c r="AD15" s="3" t="n"/>
     </row>
     <row r="16" ht="15" customHeight="1">
       <c r="A16" s="4" t="n"/>
@@ -1272,6 +1320,9 @@
       <c r="Y16" s="4" t="n"/>
       <c r="Z16" s="4" t="n"/>
       <c r="AA16" s="4" t="n"/>
+      <c r="AB16" s="4" t="n"/>
+      <c r="AC16" s="4" t="n"/>
+      <c r="AD16" s="4" t="n"/>
     </row>
     <row r="17" ht="15" customHeight="1">
       <c r="A17" s="3" t="n"/>
@@ -1301,6 +1352,9 @@
       <c r="Y17" s="3" t="n"/>
       <c r="Z17" s="3" t="n"/>
       <c r="AA17" s="3" t="n"/>
+      <c r="AB17" s="3" t="n"/>
+      <c r="AC17" s="3" t="n"/>
+      <c r="AD17" s="3" t="n"/>
     </row>
     <row r="18" ht="15" customHeight="1">
       <c r="A18" s="4" t="n"/>
@@ -1330,6 +1384,9 @@
       <c r="Y18" s="4" t="n"/>
       <c r="Z18" s="4" t="n"/>
       <c r="AA18" s="4" t="n"/>
+      <c r="AB18" s="4" t="n"/>
+      <c r="AC18" s="4" t="n"/>
+      <c r="AD18" s="4" t="n"/>
     </row>
     <row r="19" ht="15" customHeight="1">
       <c r="A19" s="3" t="n"/>
@@ -1359,6 +1416,9 @@
       <c r="Y19" s="3" t="n"/>
       <c r="Z19" s="3" t="n"/>
       <c r="AA19" s="3" t="n"/>
+      <c r="AB19" s="3" t="n"/>
+      <c r="AC19" s="3" t="n"/>
+      <c r="AD19" s="3" t="n"/>
     </row>
     <row r="20" ht="15" customHeight="1">
       <c r="A20" s="4" t="n"/>
@@ -1388,6 +1448,9 @@
       <c r="Y20" s="4" t="n"/>
       <c r="Z20" s="4" t="n"/>
       <c r="AA20" s="4" t="n"/>
+      <c r="AB20" s="4" t="n"/>
+      <c r="AC20" s="4" t="n"/>
+      <c r="AD20" s="4" t="n"/>
     </row>
     <row r="21" ht="15" customHeight="1">
       <c r="A21" s="3" t="n"/>
@@ -1417,6 +1480,9 @@
       <c r="Y21" s="3" t="n"/>
       <c r="Z21" s="3" t="n"/>
       <c r="AA21" s="3" t="n"/>
+      <c r="AB21" s="3" t="n"/>
+      <c r="AC21" s="3" t="n"/>
+      <c r="AD21" s="3" t="n"/>
     </row>
     <row r="22" ht="15" customHeight="1">
       <c r="A22" s="4" t="n"/>
@@ -1446,6 +1512,9 @@
       <c r="Y22" s="4" t="n"/>
       <c r="Z22" s="4" t="n"/>
       <c r="AA22" s="4" t="n"/>
+      <c r="AB22" s="4" t="n"/>
+      <c r="AC22" s="4" t="n"/>
+      <c r="AD22" s="4" t="n"/>
     </row>
     <row r="23" ht="15" customHeight="1">
       <c r="A23" s="3" t="n"/>
@@ -1475,6 +1544,9 @@
       <c r="Y23" s="3" t="n"/>
       <c r="Z23" s="3" t="n"/>
       <c r="AA23" s="3" t="n"/>
+      <c r="AB23" s="3" t="n"/>
+      <c r="AC23" s="3" t="n"/>
+      <c r="AD23" s="3" t="n"/>
     </row>
     <row r="24" ht="15" customHeight="1">
       <c r="A24" s="4" t="n"/>
@@ -1504,6 +1576,9 @@
       <c r="Y24" s="4" t="n"/>
       <c r="Z24" s="4" t="n"/>
       <c r="AA24" s="4" t="n"/>
+      <c r="AB24" s="4" t="n"/>
+      <c r="AC24" s="4" t="n"/>
+      <c r="AD24" s="4" t="n"/>
     </row>
     <row r="25" ht="15" customHeight="1">
       <c r="A25" s="3" t="n"/>
@@ -1533,6 +1608,9 @@
       <c r="Y25" s="3" t="n"/>
       <c r="Z25" s="3" t="n"/>
       <c r="AA25" s="3" t="n"/>
+      <c r="AB25" s="3" t="n"/>
+      <c r="AC25" s="3" t="n"/>
+      <c r="AD25" s="3" t="n"/>
     </row>
     <row r="26" ht="15" customHeight="1">
       <c r="A26" s="4" t="n"/>
@@ -1562,6 +1640,9 @@
       <c r="Y26" s="4" t="n"/>
       <c r="Z26" s="4" t="n"/>
       <c r="AA26" s="4" t="n"/>
+      <c r="AB26" s="4" t="n"/>
+      <c r="AC26" s="4" t="n"/>
+      <c r="AD26" s="4" t="n"/>
     </row>
     <row r="27" ht="15" customHeight="1">
       <c r="A27" s="3" t="n"/>
@@ -1591,6 +1672,9 @@
       <c r="Y27" s="3" t="n"/>
       <c r="Z27" s="3" t="n"/>
       <c r="AA27" s="3" t="n"/>
+      <c r="AB27" s="3" t="n"/>
+      <c r="AC27" s="3" t="n"/>
+      <c r="AD27" s="3" t="n"/>
     </row>
     <row r="28" ht="15" customHeight="1">
       <c r="A28" s="4" t="n"/>
@@ -1620,6 +1704,9 @@
       <c r="Y28" s="4" t="n"/>
       <c r="Z28" s="4" t="n"/>
       <c r="AA28" s="4" t="n"/>
+      <c r="AB28" s="4" t="n"/>
+      <c r="AC28" s="4" t="n"/>
+      <c r="AD28" s="4" t="n"/>
     </row>
     <row r="29" ht="15" customHeight="1">
       <c r="A29" s="3" t="n"/>

</xml_diff>